<commit_message>
Mistake correction in AlexNet architecture parameters
</commit_message>
<xml_diff>
--- a/Лекция 2/AlexNetComplexity.xlsx
+++ b/Лекция 2/AlexNetComplexity.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anatoly/Documents/MIET.AI.Course/Лекция 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F2151D-1813-5E45-8694-B1E325F17BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0F4444-F292-D848-A666-689DA1DFD097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="460" windowWidth="31400" windowHeight="19180" xr2:uid="{42011CF7-A167-D84A-8540-645E55F3C853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>input</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>MultAddsComp</t>
+  </si>
+  <si>
+    <t>conv5</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5CE39E-5967-304E-8064-44FF7E9C9875}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,28 +534,28 @@
         <v>55</v>
       </c>
       <c r="D3">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <f>2*E3*F3*D2*D3*B3*C3</f>
-        <v>21780000</v>
+        <v>210830400</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
         <f>E3*F3*D2*D3</f>
-        <v>3600</v>
+        <v>34848</v>
       </c>
       <c r="J3">
         <f>D3*C3*B3</f>
-        <v>145200</v>
+        <v>290400</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -566,7 +569,7 @@
         <v>55</v>
       </c>
       <c r="D4">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -580,13 +583,13 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <v>192</v>
+        <v>96</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -600,13 +603,13 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D6">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -616,18 +619,18 @@
       </c>
       <c r="G6">
         <f>2*E6*F6*D5*D6*B6*C6</f>
-        <v>112140288</v>
+        <v>322486272</v>
       </c>
       <c r="H6" s="1">
         <v>150528</v>
       </c>
       <c r="I6">
         <f>E6*F6*D5*D6</f>
-        <v>331776</v>
+        <v>221184</v>
       </c>
       <c r="J6">
         <f>D6*C6*B6</f>
-        <v>32448</v>
+        <v>186624</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -635,13 +638,13 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C7">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D7">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -652,7 +655,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>13</v>
@@ -661,33 +664,18 @@
         <v>13</v>
       </c>
       <c r="D8">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8">
         <v>3</v>
-      </c>
-      <c r="G8">
-        <f>2*E8*F8*D7*D8*B8*C8</f>
-        <v>112140288</v>
-      </c>
-      <c r="H8" s="1">
-        <v>150528</v>
-      </c>
-      <c r="I8">
-        <f>E8*F8*D7*D8</f>
-        <v>331776</v>
-      </c>
-      <c r="J8">
-        <f>D8*C8*B8</f>
-        <v>32448</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>13</v>
@@ -696,18 +684,29 @@
         <v>13</v>
       </c>
       <c r="D9">
-        <v>192</v>
+        <v>384</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
+        <v>150528</v>
+      </c>
+      <c r="I9">
+        <f>E9*F9*D7*D9</f>
+        <v>884736</v>
+      </c>
+      <c r="J9">
+        <f>D9*C9*B9</f>
+        <v>64896</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>13</v>
@@ -716,7 +715,7 @@
         <v>13</v>
       </c>
       <c r="D10">
-        <v>128</v>
+        <v>384</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -725,21 +724,13 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <f>2*E10*F10*D9*D10*B10*C10</f>
-        <v>8306688</v>
-      </c>
-      <c r="I10">
-        <f>E10*F10*D9*D10</f>
-        <v>24576</v>
-      </c>
-      <c r="J10">
-        <f>D10*C10*B10</f>
-        <v>21632</v>
+        <f>B10*C10*D10</f>
+        <v>64896</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>13</v>
@@ -748,127 +739,110 @@
         <v>13</v>
       </c>
       <c r="D11">
-        <v>192</v>
+        <v>384</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
+      </c>
+      <c r="I11">
+        <f>E11*F11*D10*D11</f>
+        <v>147456</v>
+      </c>
+      <c r="J11">
+        <f>D11*C11*B11</f>
+        <v>64896</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D12">
-        <v>4096</v>
+        <v>384</v>
       </c>
       <c r="E12">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>13</v>
-      </c>
-      <c r="G12">
-        <f>2*E12*F12*D11*D12*B12*C12</f>
-        <v>265814016</v>
-      </c>
-      <c r="H12" s="1">
-        <v>150528</v>
-      </c>
-      <c r="I12">
-        <f>E12*F12*D11*D12</f>
-        <v>132907008</v>
-      </c>
-      <c r="J12">
-        <f>D12*C12*B12</f>
-        <v>4096</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D13">
-        <v>1000</v>
+        <v>256</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <f>2*E13*F13*D12*D13*B13*C13</f>
+        <v>299040768</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D14">
-        <v>4096</v>
+        <v>256</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
         <v>1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>21780000</v>
-      </c>
-      <c r="H14" s="1">
-        <v>150528</v>
-      </c>
-      <c r="I14">
-        <f>E14*F14*D13*D14</f>
-        <v>4096000</v>
-      </c>
-      <c r="J14">
-        <f>D14*C14*B14</f>
-        <v>4096</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>4096</v>
+        <v>256</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -877,32 +851,33 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>1000</v>
+        <v>4096</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1">
-        <v>21780000</v>
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <f>2*E16*F16*D12*D16*B16*C16</f>
+        <v>531628032</v>
       </c>
       <c r="H16" s="1">
         <v>150528</v>
       </c>
       <c r="I16">
-        <f>E16*F16*D15*D16</f>
-        <v>4096000</v>
+        <f>E16*F16*D12*D16</f>
+        <v>265814016</v>
       </c>
       <c r="J16">
         <f>D16*C16*B16</f>
-        <v>1000</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -922,29 +897,137 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>4096</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>21780000</v>
+      </c>
+      <c r="H18" s="1">
+        <v>150528</v>
+      </c>
+      <c r="I18">
+        <f>E18*F18*D17*D18</f>
+        <v>4096000</v>
+      </c>
+      <c r="J18">
+        <f>D18*C18*B18</f>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>4096</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1000</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>21780000</v>
+      </c>
+      <c r="H20" s="1">
+        <v>150528</v>
+      </c>
+      <c r="I20">
+        <f>E20*F20*D19*D20</f>
+        <v>4096000</v>
+      </c>
+      <c r="J20">
+        <f>D20*C20*B20</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1000</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="2">
-        <f>SUM(G2:G17)</f>
-        <v>563741280</v>
-      </c>
-      <c r="H18">
-        <f>SUM(H2:H17)</f>
+      <c r="G22" s="2">
+        <f>SUM(G2:G21)</f>
+        <v>1407610368</v>
+      </c>
+      <c r="H22">
+        <f>SUM(H2:H21)</f>
         <v>903168</v>
       </c>
-      <c r="I18">
-        <f>SUM(I2:I17)</f>
-        <v>141790736</v>
-      </c>
-      <c r="J18">
-        <f>SUM(J2:J17)</f>
-        <v>240920</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H19">
-        <f>SUM(H18:J18)/4/1024/1024</f>
-        <v>34.078317642211914</v>
+      <c r="I22">
+        <f>SUM(I2:I21)</f>
+        <v>275294240</v>
+      </c>
+      <c r="J22">
+        <f>SUM(J2:J21)</f>
+        <v>616008</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <f>SUM(H22:J22)/4/1024/1024</f>
+        <v>65.997461318969727</v>
       </c>
     </row>
   </sheetData>

</xml_diff>